<commit_message>
Update script.js 2nd time with change in tablet number
</commit_message>
<xml_diff>
--- a/Work_LogSheet.xlsx
+++ b/Work_LogSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8657b17cc784b9aa/Desktop/ServiceLearning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{866411D5-1DEE-4AAD-9C62-6970278CBB32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{866411D5-1DEE-4AAD-9C62-6970278CBB32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B8915E1-A2C5-4BC8-BB53-4F336600C0B1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{42E264D9-AFBF-4B3F-9995-479FC89D7096}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>week 1</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t xml:space="preserve">researched on possible solutions for the problem statement. Made a questionanaire to standardize learning for the nurses. Developed a prototype for inventory. </t>
+  </si>
+  <si>
+    <t>week 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">observed the HMI system. Took insights . Brainstromed solution for inventory mangement. Developed basic logic for Pill distribution . </t>
   </si>
 </sst>
 </file>
@@ -162,7 +168,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -185,9 +191,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -209,6 +212,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -531,7 +538,7 @@
   <dimension ref="A2:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,7 +554,7 @@
       </c>
       <c r="L2" s="9">
         <f>SUM(I5:I37)</f>
-        <v>8.0000000000000036</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
@@ -566,7 +573,7 @@
       <c r="E4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="5" t="s">
@@ -629,22 +636,44 @@
         <v>17</v>
       </c>
       <c r="G6" s="7">
-        <v>0.54166666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="H6" s="7">
-        <v>0.70833333333333337</v>
+        <v>0.75</v>
       </c>
       <c r="I6" s="8">
         <f t="shared" ref="I6:I40" si="0">(H6-G6)*24</f>
-        <v>4.0000000000000018</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1">
+        <v>45863</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="I7" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.9999999999999991</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>